<commit_message>
Added memory usage chart for S1
</commit_message>
<xml_diff>
--- a/bench/results/jmeter_S1_analysis.xlsx
+++ b/bench/results/jmeter_S1_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\corey\Documents\GitHub\Honours-Project\bench\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10000001_{7B4F5FD3-0759-43C4-B678-F5E7792FA632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B4D6FC-A6A5-4FBD-87E3-9974EE4653B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3480" windowWidth="38640" windowHeight="21120" tabRatio="117" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>Framework</t>
   </si>
@@ -78,6 +77,9 @@
   <si>
     <t>Throughput vs Concurrent Users (Scenario 1)</t>
   </si>
+  <si>
+    <t>Apache HTTP Server Memory Usage (MB) (Scenario 1)</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +117,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +133,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -170,6 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2495,7 +2504,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2854,7 +2863,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3167,6 +3175,752 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Apache HTTP Server Memory Usage (MB</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>) (Scenario 1)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Laravel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$22:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$22:$P$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-667E-47CC-B0BC-6B40DA6FA420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CodeIgniter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$22:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$22:$Q$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-667E-47CC-B0BC-6B40DA6FA420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Symfony</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$22:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$22:$R$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-667E-47CC-B0BC-6B40DA6FA420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yii</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$O$22:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$22:$S$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-667E-47CC-B0BC-6B40DA6FA420}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="683390207"/>
+        <c:axId val="683390687"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="683390207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Concurrent Users</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="683390687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="683390687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Usage (MB/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="683390207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3327,6 +4081,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -4837,6 +5631,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5387,8 +6684,8 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>280147</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5480,6 +6777,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>911088</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>11596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>8284</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>87796</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2C8D4AC-AA93-7753-0766-405F05628362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5753,8 +7086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5769,6 +7102,9 @@
     <col min="11" max="11" width="14.140625" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
     <col min="19" max="19" width="14.42578125" customWidth="1"/>
     <col min="27" max="27" width="14.42578125" customWidth="1"/>
   </cols>
@@ -6366,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -6389,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -6412,12 +7748,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I20" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="O20" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="1" t="s">
         <v>1</v>
       </c>
@@ -6433,8 +7772,23 @@
       <c r="M21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="O21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I22" s="2">
         <v>1</v>
       </c>
@@ -6450,8 +7804,23 @@
       <c r="M22" s="2">
         <v>14.925369999999999</v>
       </c>
+      <c r="O22" s="7">
+        <v>1</v>
+      </c>
+      <c r="P22" s="7">
+        <v>35</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="R22" s="7">
+        <v>30.5</v>
+      </c>
+      <c r="S22" s="7">
+        <v>28.9</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="2">
         <v>10</v>
       </c>
@@ -6467,8 +7836,23 @@
       <c r="M23" s="2">
         <v>1.1050899999999999</v>
       </c>
+      <c r="O23" s="7">
+        <v>10</v>
+      </c>
+      <c r="P23" s="7">
+        <v>36.5</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>29.4</v>
+      </c>
+      <c r="R23" s="7">
+        <v>32.6</v>
+      </c>
+      <c r="S23" s="7">
+        <v>29.6</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="2">
         <v>50</v>
       </c>
@@ -6484,8 +7868,23 @@
       <c r="M24" s="2">
         <v>1.01912</v>
       </c>
+      <c r="O24" s="7">
+        <v>50</v>
+      </c>
+      <c r="P24" s="7">
+        <v>37.5</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>30.5</v>
+      </c>
+      <c r="R24" s="7">
+        <v>32.6</v>
+      </c>
+      <c r="S24" s="7">
+        <v>29.8</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="2">
         <v>100</v>
       </c>
@@ -6500,6 +7899,21 @@
       </c>
       <c r="M25" s="2">
         <v>1.0095400000000001</v>
+      </c>
+      <c r="O25" s="7">
+        <v>100</v>
+      </c>
+      <c r="P25" s="7">
+        <v>38.5</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>31</v>
+      </c>
+      <c r="R25" s="7">
+        <v>34</v>
+      </c>
+      <c r="S25" s="7">
+        <v>30.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>